<commit_message>
Link User with SinhVien/GiangVien when logging in
</commit_message>
<xml_diff>
--- a/server/sinhViens.xlsx
+++ b/server/sinhViens.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\QuanLyKhoaLuan\quan-ly-khoa-luan\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB151EE8-B197-43C9-8437-999824CA3AF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FB6980-D327-410D-9B30-95A18EB99B0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>maSV</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Nguyễn Văn E</t>
+  </si>
+  <si>
+    <t>16521178</t>
+  </si>
+  <si>
+    <t>Nguyễn Đình Phú Thịnh</t>
+  </si>
+  <si>
+    <t>0383965078</t>
+  </si>
+  <si>
+    <t>16521178@gm.uit.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -438,11 +450,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -575,6 +585,26 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -587,6 +617,8 @@
     <hyperlink ref="F5" r:id="rId7" xr:uid="{FBCD616D-6BB0-4DEE-9506-C7865A6B398F}"/>
     <hyperlink ref="D6" r:id="rId8" xr:uid="{C615ACE8-E0BC-490A-AC74-87A5D47DA04F}"/>
     <hyperlink ref="F6" r:id="rId9" xr:uid="{77020DD5-6C64-482B-B244-EBBF589791C1}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{797E824F-5F1A-46E5-8DC4-91BC1ED77243}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{233B132B-0A3B-45F4-B7CA-58D2B287AB60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>